<commit_message>
!201 岗位管理 * Merge branch 'dev' of https://gitee.com/fxzcloud/pig into dev * :sparkles: 岗位管理
</commit_message>
<xml_diff>
--- a/pig-upms/pig-upms-biz/src/main/resources/file/user.xlsx
+++ b/pig-upms/pig-upms-biz/src/main/resources/file/user.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lengleng/work/open/pig/pig-upms/pig-upms-biz/src/main/resources/file/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF1A8A-DAD5-654E-937C-BA9E399F26C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="22368" windowHeight="9575"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>用户名</t>
   </si>
@@ -34,37 +28,189 @@
     <t>角色</t>
   </si>
   <si>
+    <t>岗位</t>
+  </si>
+  <si>
     <t>锁定标记,0:正常,9:已锁定</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,10 +220,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -100,9 +433,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -114,17 +689,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -173,7 +792,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -206,26 +825,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -258,23 +860,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -416,29 +1001,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="13.8" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="26.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" ht="34.8" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,9 +1035,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>